<commit_message>
modify:basic 5 stage pipeline without forward and stall
</commit_message>
<xml_diff>
--- a/instr.xlsx
+++ b/instr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WZH\Desktop\coding\CPU\Basic_5_Stage_pipeline_CPU(Xilinx_Artrix7)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80272E1-53F5-4552-B026-51611B3E67D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDB0877-8B39-4EA4-A161-8FCA4A1F0BBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="2280" windowWidth="22530" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="75">
   <si>
     <t>instr</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>imm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_new</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rs_use</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rt_use</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -400,18 +412,18 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -698,714 +710,741 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ46"/>
+  <dimension ref="A1:AT46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="8.6640625" style="1"/>
-    <col min="6" max="6" width="10.4140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.58203125" style="1" customWidth="1"/>
-    <col min="9" max="43" width="8.6640625" style="1"/>
+    <col min="4" max="8" width="8.6640625" style="1"/>
+    <col min="9" max="9" width="10.4140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.25" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.58203125" style="1" customWidth="1"/>
+    <col min="12" max="46" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="F17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E24" s="2" t="s">
+    <row r="24" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="H24" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C25" s="3" t="s">
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="F25" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="E26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="F26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="G26" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="H26" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="I26" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="J26" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="I28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" s="1" t="s">
+      <c r="I30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="1" t="s">
+      <c r="F31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="F32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="F33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="I34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="I35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="1" t="s">
+      <c r="I36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="I37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="I38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D39" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F39" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="I39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D40" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D41" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D42" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D43" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D44" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D45" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="G45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J45" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D46" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="H24:J24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>